<commit_message>
basic control logic working
</commit_message>
<xml_diff>
--- a/docs/SPAM1-AVR-Like.xlsx
+++ b/docs/SPAM1-AVR-Like.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/db8094ce4aaa691d/simplecpu/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E355E389-9FB3-4E8C-984E-0F784E421D7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="722" documentId="8_{E355E389-9FB3-4E8C-984E-0F784E421D7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{81650D60-A390-4370-AE38-1D3A2E243F85}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" activeTab="3" xr2:uid="{B4484DA9-D572-4854-B84C-0917FAD72649}"/>
   </bookViews>
@@ -18,6 +18,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="AVR like" sheetId="5" r:id="rId4"/>
     <sheet name="WriteDecoder" sheetId="2" r:id="rId5"/>
+    <sheet name="ControlDecode" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1431" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="275">
   <si>
     <t>PCLOin</t>
   </si>
@@ -435,15 +436,6 @@
     <t>reg to ram[MAR]</t>
   </si>
   <si>
-    <t>JMPOF</t>
-  </si>
-  <si>
-    <t>JMPZS</t>
-  </si>
-  <si>
-    <t>JMPCS</t>
-  </si>
-  <si>
     <t>JMPDI</t>
   </si>
   <si>
@@ -453,9 +445,6 @@
     <t>Jump if overflow</t>
   </si>
   <si>
-    <t>Jump in page if Carry set</t>
-  </si>
-  <si>
     <t>Jump if Data In ready</t>
   </si>
   <si>
@@ -465,18 +454,6 @@
     <t>sets REGin and REGW value</t>
   </si>
   <si>
-    <t>NOOP useful for CMP operation which just sets flags</t>
-  </si>
-  <si>
-    <t>set HI byte - doesn't cause jump</t>
-  </si>
-  <si>
-    <t>Jump in page if Zero set</t>
-  </si>
-  <si>
-    <t>JMPPAGEin</t>
-  </si>
-  <si>
     <t>MAR=1</t>
   </si>
   <si>
@@ -648,9 +625,6 @@
     <t>write to a reg</t>
   </si>
   <si>
-    <t>DEST</t>
-  </si>
-  <si>
     <t>WRITE DEST</t>
   </si>
   <si>
@@ -681,32 +655,176 @@
     <t>Jump unconditionally</t>
   </si>
   <si>
-    <t>to [JMPPAGE,Bus]</t>
-  </si>
-  <si>
-    <t>Bits [d,c,b,a] defines first operand of ALU op X in ...      X=X OP Y</t>
-  </si>
-  <si>
-    <t>JMPLOC</t>
-  </si>
-  <si>
-    <t>Jump local unconditional</t>
-  </si>
-  <si>
-    <t>to [=,Bus]</t>
-  </si>
-  <si>
     <t>See long decoding : http://www.ti.com/lit/ds/symlink/cd74act138.pdf</t>
   </si>
   <si>
     <t>74hct138*2  - Inverting 3 to 8 decoder  PLUS 1 Inverter</t>
   </si>
   <si>
-    <t>AND WITH CONTROL LINE</t>
+    <t>DEVICE=ROM</t>
+  </si>
+  <si>
+    <t>PGZERO</t>
+  </si>
+  <si>
+    <t>REGY</t>
+  </si>
+  <si>
+    <t>REGX</t>
+  </si>
+  <si>
+    <t>DEVICE=UART</t>
+  </si>
+  <si>
+    <t>RAM[PGZERO]=UART</t>
+  </si>
+  <si>
+    <t>RAM[MAR]=UART</t>
+  </si>
+  <si>
+    <t>DEV=ROM</t>
+  </si>
+  <si>
+    <t>DEV=RAM[ZP]</t>
+  </si>
+  <si>
+    <t>DEV=RAM[MAR]</t>
+  </si>
+  <si>
+    <t>DEV=UART</t>
+  </si>
+  <si>
+    <t>RAM[ZP]=UART</t>
+  </si>
+  <si>
+    <t>REGX=ALU(REGX,REGY)</t>
+  </si>
+  <si>
+    <t>IDX MODE</t>
+  </si>
+  <si>
+    <t>BUS_ACC</t>
+  </si>
+  <si>
+    <t>ROM</t>
+  </si>
+  <si>
+    <t>MULTIPLEX</t>
+  </si>
+  <si>
+    <t>ALSO</t>
+  </si>
+  <si>
+    <t>BUS_CTL</t>
+  </si>
+  <si>
+    <t>WRITE_EN</t>
+  </si>
+  <si>
+    <t>MAR_TO_RAM_ADDR=OFF</t>
+  </si>
+  <si>
+    <t>ROM_TO_RAM_ADDR_LO=ON</t>
+  </si>
+  <si>
+    <t>MAR_TO_RAM_ADDR=ON</t>
+  </si>
+  <si>
+    <t>ALUOP=PASSA</t>
+  </si>
+  <si>
+    <t>RAM[ZP]=PASSA(REGX)</t>
+  </si>
+  <si>
+    <t>RAM[MAR]=PASSA(REGX)</t>
+  </si>
+  <si>
+    <t>ALUOP=BITS[ALUOP]</t>
+  </si>
+  <si>
+    <t>DEVICE=RAM[MAR]</t>
+  </si>
+  <si>
+    <t>DEVICE=RAM[ZP]</t>
+  </si>
+  <si>
+    <t>to [PCHI,Bus]</t>
+  </si>
+  <si>
+    <t>BUS OUT</t>
+  </si>
+  <si>
+    <t>Implies ROM_OVERRIDE_MAR_LO &amp; MAR_HI=0</t>
+  </si>
+  <si>
+    <t>RAM_ZP_out</t>
+  </si>
+  <si>
+    <t>ZP_MODE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">implies write RAM select ZP, ALUOP=PASSX </t>
+  </si>
+  <si>
+    <t>ROM_TO_DEVICE</t>
+  </si>
+  <si>
+    <t>RAM[MAR]_TO_DEVICE</t>
+  </si>
+  <si>
+    <t>RAM[ZP]_TO_DEVICE</t>
+  </si>
+  <si>
+    <t>JMPEQ</t>
+  </si>
+  <si>
+    <t>JMPNE</t>
+  </si>
+  <si>
+    <t>JMPGT</t>
+  </si>
+  <si>
+    <t>JMPLT</t>
+  </si>
+  <si>
+    <t>also use as NOOP?</t>
+  </si>
+  <si>
+    <t>local page jump</t>
+  </si>
+  <si>
+    <t>to [PCHITMPin,Bus]</t>
+  </si>
+  <si>
+    <t>/EN =  74138(E3=1,/E2=E,/E1=D,A2=C,A1=B,A0=A)</t>
+  </si>
+  <si>
+    <t>/EN =  74138(E3=D,/E2=E,/E1=0,A2=C,A1=B,A0=A)</t>
+  </si>
+  <si>
+    <t>Jump local page absolute</t>
+  </si>
+  <si>
+    <t>JMPO</t>
+  </si>
+  <si>
+    <t>JMPZ</t>
+  </si>
+  <si>
+    <t>JMPC</t>
+  </si>
+  <si>
+    <t>Jump if Zero set</t>
+  </si>
+  <si>
+    <t>Jump if Carry set</t>
+  </si>
+  <si>
+    <t>If want CMP operator then do REGX=PASSA(REGX, REGY) ie NOOP, we still get the magnitude outputs</t>
   </si>
   <si>
     <r>
-      <t>/REG EN LINE =  74138(E3=1,</t>
+      <t>/REG W =</t>
     </r>
     <r>
       <rPr>
@@ -717,80 +835,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>/E2=NOR(F,E),/E1=D,A2=C,A1=B,A0=A</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>/JMP EN LINE =  74138(</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>E3=D,/E2=NOR(F,E)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,/E1=0,</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>A2=C,A1=B,A0=A</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>REG W =</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> NOR(F, NOT E)</t>
+      <t xml:space="preserve"> NOT E</t>
     </r>
     <r>
       <rPr>
@@ -804,101 +849,46 @@
     </r>
   </si>
   <si>
-    <t>DEVICE=ROM</t>
-  </si>
-  <si>
-    <t>PGZERO</t>
-  </si>
-  <si>
-    <t>OP</t>
-  </si>
-  <si>
-    <t>DEVICE=ram out[#0-255]</t>
-  </si>
-  <si>
-    <t>DEVICE=ram out[MAR]</t>
-  </si>
-  <si>
-    <t>REGX=ALUOP(REGX,REGY)</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>REGY</t>
-  </si>
-  <si>
-    <t>REGX</t>
-  </si>
-  <si>
-    <t>DEVICE=UART</t>
-  </si>
-  <si>
-    <t>RAM[PGZERO]=UART</t>
-  </si>
-  <si>
-    <t>RAM[MAR]=UART</t>
-  </si>
-  <si>
-    <t>RAM[ZP]=PASS(REGX)</t>
-  </si>
-  <si>
-    <t>RAM[MAR]=PASS(REGX)</t>
-  </si>
-  <si>
-    <t>DEV=ROM</t>
-  </si>
-  <si>
-    <t>DEV=RAM[ZP]</t>
-  </si>
-  <si>
-    <t>DEV=RAM[MAR]</t>
-  </si>
-  <si>
-    <t>DEV=UART</t>
-  </si>
-  <si>
-    <t>RAM[ZP]=UART</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>REGX=ALU(REGX,REGY)</t>
-  </si>
-  <si>
-    <t>Bit2 relevant only when writing to RAM 00011</t>
-  </si>
-  <si>
-    <t>When ALU_OUT then decoder bit E is always 1  thereofr but 2 &amp; 3 of opcode can be additional decoding for where result gets written : Bit3 ? 1 means back to REGX, 0 means to RAM,  Bit2: RamIndex mode</t>
-  </si>
-  <si>
-    <t>IDX MODE</t>
-  </si>
-  <si>
-    <t>MAR/ZP determined elsewhere</t>
-  </si>
-  <si>
-    <t>RAM[MAR]=ALUOP(REGX,REGY)</t>
-  </si>
-  <si>
-    <t>UART=ALUOP(REGX,REGY)</t>
+    <t>noop: A=A</t>
+  </si>
+  <si>
+    <t>REGX=ALU(ALUOP,REGX,REGY)</t>
+  </si>
+  <si>
+    <t>RAM[ZP]=ALU("A", REGX, xxxx[ignored so could be PGZERO bit])</t>
+  </si>
+  <si>
+    <t>REGY address can always be these 4 bits</t>
+  </si>
+  <si>
+    <t>Not useful as we don't have ZPAddress</t>
+  </si>
+  <si>
+    <t>ALUOP always wired to these 4 bits</t>
+  </si>
+  <si>
+    <t>PZ Buffer always wired to these 8 bits …............................................</t>
+  </si>
+  <si>
+    <t>RegX address always wired to these 4 pins</t>
+  </si>
+  <si>
+    <t>implies select ZP</t>
   </si>
   <si>
     <r>
-      <t>RAM[ZP]=</t>
+      <t xml:space="preserve">implies calc written back to reg </t>
     </r>
     <r>
       <rPr>
         <b/>
-        <i/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>PASS</t>
+      <t xml:space="preserve">therefore </t>
     </r>
     <r>
       <rPr>
@@ -908,15 +898,47 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(REGX)</t>
+      <t xml:space="preserve">  REG_in=enable</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">means save calc to device other than reg </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>therefore</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> REG_in=disable &amp; REGX value must be constant 0 - put a pull down on the REGX bus and then disable all register outs</t>
+    </r>
+  </si>
+  <si>
+    <t>NONREG=ALU(ALUOP,0,REGY)</t>
+  </si>
+  <si>
+    <t>implies OVERRIDE device and use write RAM, ZP=enable, ALUOP=PASSX (alu op 1),  REG_in=disable,</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -944,15 +966,6 @@
       <color theme="1"/>
       <name val="Courier New"/>
       <family val="3"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -988,7 +1001,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1413,7 +1426,7 @@
         <v>0</v>
       </c>
       <c r="K8" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -1439,7 +1452,7 @@
         <v>3</v>
       </c>
       <c r="K9" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -1465,7 +1478,7 @@
         <v>8</v>
       </c>
       <c r="K10" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -1488,10 +1501,10 @@
         <v>1</v>
       </c>
       <c r="I11" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="K11" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -1505,10 +1518,10 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="K12" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -1525,7 +1538,7 @@
         <v>4</v>
       </c>
       <c r="K13" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -1542,7 +1555,7 @@
         <v>5</v>
       </c>
       <c r="K14" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -1849,7 +1862,7 @@
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B26" t="s">
         <v>22</v>
@@ -1873,7 +1886,7 @@
         <v>21</v>
       </c>
       <c r="I26" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="J26" t="s">
         <v>23</v>
@@ -1926,7 +1939,7 @@
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="B27" t="s">
         <v>22</v>
@@ -1950,7 +1963,7 @@
         <v>21</v>
       </c>
       <c r="I27" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="J27" t="s">
         <v>23</v>
@@ -2157,7 +2170,7 @@
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B31" t="s">
         <v>24</v>
@@ -2388,7 +2401,7 @@
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="B35" t="s">
         <v>51</v>
@@ -2619,7 +2632,7 @@
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="B40" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.55000000000000004">
@@ -2627,13 +2640,13 @@
         <v>0</v>
       </c>
       <c r="B41" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="D41" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="E41" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="I41" t="s">
         <v>120</v>
@@ -2647,10 +2660,10 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E42" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="I42" t="s">
         <v>43</v>
@@ -2670,7 +2683,7 @@
         <v>2</v>
       </c>
       <c r="B43" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="I43" t="s">
         <v>44</v>
@@ -2679,10 +2692,10 @@
         <v>8</v>
       </c>
       <c r="L43" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="M43" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.55000000000000004">
@@ -2690,22 +2703,22 @@
         <v>3</v>
       </c>
       <c r="B44" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="E44" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="I44" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="J44">
         <v>4</v>
       </c>
       <c r="L44" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="M44" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.55000000000000004">
@@ -2713,22 +2726,22 @@
         <v>4</v>
       </c>
       <c r="B45" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="E45" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="I45" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="J45">
         <v>1</v>
       </c>
       <c r="L45" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="M45" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.55000000000000004">
@@ -2744,10 +2757,10 @@
         <v>2097152</v>
       </c>
       <c r="L46" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="M46" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.55000000000000004">
@@ -2755,16 +2768,16 @@
         <v>6</v>
       </c>
       <c r="B47" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D47" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="L47" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="M47" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
     </row>
     <row r="48" spans="1:25" x14ac:dyDescent="0.55000000000000004">
@@ -2772,16 +2785,16 @@
         <v>7</v>
       </c>
       <c r="B48" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D48" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="L48" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="M48" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
     </row>
     <row r="49" spans="1:25" x14ac:dyDescent="0.55000000000000004">
@@ -2789,16 +2802,16 @@
         <v>8</v>
       </c>
       <c r="B49" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="D49" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="L49" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="M49" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
     </row>
     <row r="50" spans="1:25" x14ac:dyDescent="0.55000000000000004">
@@ -2806,10 +2819,10 @@
         <v>9</v>
       </c>
       <c r="B50" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D50" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
     </row>
     <row r="51" spans="1:25" x14ac:dyDescent="0.55000000000000004">
@@ -2817,10 +2830,10 @@
         <v>10</v>
       </c>
       <c r="B51" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="D51" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
     </row>
     <row r="52" spans="1:25" x14ac:dyDescent="0.55000000000000004">
@@ -2828,10 +2841,10 @@
         <v>11</v>
       </c>
       <c r="B52" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="E52" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
     </row>
     <row r="53" spans="1:25" x14ac:dyDescent="0.55000000000000004">
@@ -2839,10 +2852,10 @@
         <v>12</v>
       </c>
       <c r="B53" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="E53" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
     </row>
     <row r="54" spans="1:25" x14ac:dyDescent="0.55000000000000004">
@@ -2850,7 +2863,7 @@
         <v>13</v>
       </c>
       <c r="B54" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
     </row>
     <row r="55" spans="1:25" x14ac:dyDescent="0.55000000000000004">
@@ -2858,7 +2871,7 @@
         <v>14</v>
       </c>
       <c r="B55" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
     </row>
     <row r="56" spans="1:25" x14ac:dyDescent="0.55000000000000004">
@@ -2866,15 +2879,15 @@
         <v>15</v>
       </c>
       <c r="B56" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
     </row>
     <row r="59" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="L59" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="O59" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
     </row>
     <row r="61" spans="1:25" x14ac:dyDescent="0.55000000000000004">
@@ -3162,7 +3175,7 @@
     </row>
     <row r="67" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="B67" t="s">
         <v>22</v>
@@ -3186,36 +3199,36 @@
         <v>23</v>
       </c>
       <c r="I67" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="J67" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="K67" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="L67" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="M67" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="N67" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="O67" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="P67" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="Q67" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
     </row>
     <row r="68" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="B68" t="s">
         <v>22</v>
@@ -3239,7 +3252,7 @@
         <v>23</v>
       </c>
       <c r="I68" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="J68" t="s">
         <v>23</v>
@@ -3319,7 +3332,7 @@
         <v>16</v>
       </c>
       <c r="AA70" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
     </row>
     <row r="71" spans="1:27" x14ac:dyDescent="0.55000000000000004">
@@ -3377,7 +3390,7 @@
     </row>
     <row r="72" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B72" t="s">
         <v>24</v>
@@ -3536,7 +3549,7 @@
     </row>
     <row r="76" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="B76" t="s">
         <v>51</v>
@@ -5335,2075 +5348,794 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED8E6E0D-D3C4-4F44-A896-D8576BD5D307}">
-  <dimension ref="A2:AA76"/>
+  <dimension ref="A1:Q51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.26171875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="29.05078125" customWidth="1"/>
-    <col min="10" max="10" width="7.5234375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.68359375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.68359375" customWidth="1"/>
+    <col min="2" max="17" width="8.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="F1" t="s">
+        <v>269</v>
+      </c>
+      <c r="J1" t="s">
+        <v>267</v>
+      </c>
+      <c r="N1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="J2" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4" s="5">
+        <v>7</v>
+      </c>
+      <c r="K4" s="5">
+        <v>6</v>
+      </c>
+      <c r="L4" s="5">
+        <v>5</v>
+      </c>
+      <c r="M4" s="5">
+        <v>4</v>
+      </c>
+      <c r="N4" s="5">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" t="s">
-        <v>8</v>
-      </c>
-      <c r="R2" t="s">
-        <v>7</v>
-      </c>
-      <c r="S2" t="s">
-        <v>9</v>
-      </c>
-      <c r="T2" t="s">
-        <v>10</v>
-      </c>
-      <c r="U2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="O4" s="5">
+        <v>2</v>
+      </c>
+      <c r="P4" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="O5" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P5" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q5" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q6" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.55000000000000004">
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="K8" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.55000000000000004">
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="I9" t="s">
-        <v>3</v>
-      </c>
-      <c r="K9" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.55000000000000004">
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10" t="s">
-        <v>8</v>
-      </c>
-      <c r="K10" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.55000000000000004">
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="I11" t="s">
-        <v>194</v>
-      </c>
-      <c r="K11" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.55000000000000004">
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12" t="s">
-        <v>195</v>
-      </c>
-      <c r="K12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.55000000000000004">
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-      <c r="I13" t="s">
-        <v>4</v>
-      </c>
-      <c r="K13" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.55000000000000004">
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14" t="s">
-        <v>5</v>
-      </c>
-      <c r="K14" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.55000000000000004">
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="H15">
-        <v>1</v>
-      </c>
-      <c r="I15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="10">
+        <v>1</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>234</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q10" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>235</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="10">
+        <v>1</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="P11" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="Q11" s="5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="B15" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.55000000000000004">
-      <c r="S18">
-        <v>0</v>
-      </c>
-      <c r="T18" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.55000000000000004">
-      <c r="S19">
-        <v>1</v>
-      </c>
-      <c r="T19" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.55000000000000004">
-      <c r="B20">
-        <v>0</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20">
-        <v>2</v>
-      </c>
-      <c r="E20">
-        <v>3</v>
-      </c>
-      <c r="F20">
-        <v>4</v>
-      </c>
-      <c r="G20">
-        <v>5</v>
-      </c>
-      <c r="H20">
-        <v>6</v>
-      </c>
-      <c r="I20">
-        <v>7</v>
-      </c>
-      <c r="J20" s="5">
-        <v>0</v>
-      </c>
-      <c r="K20" s="5">
-        <v>1</v>
-      </c>
-      <c r="L20" s="5">
-        <v>2</v>
-      </c>
-      <c r="M20" s="5">
-        <v>3</v>
-      </c>
-      <c r="N20" s="5">
-        <v>4</v>
-      </c>
-      <c r="O20" s="5">
-        <v>5</v>
-      </c>
-      <c r="P20" s="5">
-        <v>6</v>
-      </c>
-      <c r="Q20" s="5">
-        <v>7</v>
-      </c>
-      <c r="S20">
-        <v>2</v>
-      </c>
-      <c r="T20" t="s">
+        <v>273</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16" s="9">
+        <v>0</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N16" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="O16" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="P16" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="Q16" s="5" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="B17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>263</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18" s="9">
+        <v>1</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L18" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M18" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N18" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="O18" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="P18" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="Q18" s="5" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="B19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
+        <v>264</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="10">
+        <v>1</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="L20" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="M20" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="N20" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="O20" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="P20" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="Q20" s="5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="B21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="D24" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" t="s">
+        <v>211</v>
+      </c>
+      <c r="B25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25" t="s">
+        <v>101</v>
+      </c>
+      <c r="F25" t="s">
+        <v>101</v>
+      </c>
+      <c r="G25" t="s">
+        <v>101</v>
+      </c>
+      <c r="H25" t="s">
+        <v>101</v>
+      </c>
+      <c r="I25" t="s">
+        <v>101</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L25" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M25" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="N25" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="O25" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P25" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q25" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" t="s">
+        <v>213</v>
+      </c>
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K26" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L26" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M26" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="N26" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="O26" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P26" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q26" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" t="s">
+        <v>212</v>
+      </c>
+      <c r="B27" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="10">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="K27" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="L27" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="M27" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="N27" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="O27" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="P27" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="Q27" s="5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.55000000000000004">
-      <c r="B21" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="J21" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="K21" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="L21" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="M21" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="N21" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="O21" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="P21" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q21" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="S21">
-        <v>3</v>
-      </c>
-      <c r="T21" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" t="s">
-        <v>225</v>
-      </c>
-      <c r="B22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22" t="s">
-        <v>231</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="I22" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="J22" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K22" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L22" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="M22" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="N22" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="O22" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="P22" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q22" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="S22">
-        <v>4</v>
-      </c>
-      <c r="T22" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.55000000000000004">
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="5"/>
-      <c r="O23" s="5"/>
-      <c r="P23" s="5"/>
-      <c r="Q23" s="5"/>
-      <c r="S23">
-        <v>5</v>
-      </c>
-      <c r="T23" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" t="s">
-        <v>228</v>
-      </c>
-      <c r="B24" t="s">
-        <v>22</v>
-      </c>
-      <c r="C24" t="s">
-        <v>22</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="H24" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="I24" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="J24" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="K24" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="L24" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="M24" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="N24" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="O24" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="P24" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="Q24" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="S24">
-        <v>6</v>
-      </c>
-      <c r="T24" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" t="s">
-        <v>229</v>
-      </c>
-      <c r="B25" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" t="s">
-        <v>22</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="F25" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="H25" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="I25" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="J25" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="K25" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="L25" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="M25" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="N25" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="O25" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="P25" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q25" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="S25">
-        <v>7</v>
-      </c>
-      <c r="T25" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.55000000000000004">
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="5"/>
-      <c r="N26" s="5"/>
-      <c r="O26" s="5"/>
-      <c r="P26" s="5"/>
-      <c r="Q26" s="5"/>
-      <c r="S26">
-        <v>8</v>
-      </c>
-      <c r="T26" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" t="s">
-        <v>247</v>
-      </c>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="5"/>
-      <c r="N27" s="5"/>
-      <c r="O27" s="5"/>
-      <c r="P27" s="5"/>
-      <c r="Q27" s="5"/>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" t="s">
-        <v>230</v>
-      </c>
-      <c r="B28" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28" t="s">
-        <v>24</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="G28" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="H28" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="I28" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="J28" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="K28" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="L28" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="M28" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="N28" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="O28" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="P28" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="Q28" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="S28">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" t="s">
-        <v>252</v>
-      </c>
-      <c r="B29" t="s">
-        <v>24</v>
-      </c>
-      <c r="C29" t="s">
-        <v>24</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>1</v>
-      </c>
-      <c r="F29" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="G29" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="H29" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="I29" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="J29" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="K29" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="L29" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="M29" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="N29" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="O29" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="P29" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="Q29" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="S29" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" t="s">
-        <v>250</v>
-      </c>
-      <c r="B30" t="s">
-        <v>24</v>
-      </c>
-      <c r="C30" t="s">
-        <v>24</v>
-      </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="F30" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="G30" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="H30" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="I30" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="J30" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="K30" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="L30" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="M30" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="N30" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="O30" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="P30" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="Q30" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="S30" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" t="s">
-        <v>251</v>
-      </c>
-      <c r="B31" t="s">
-        <v>24</v>
-      </c>
-      <c r="C31" t="s">
-        <v>24</v>
-      </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="E31">
-        <v>1</v>
-      </c>
-      <c r="F31" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="G31" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="H31" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="I31" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="J31" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="K31" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="L31" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="M31" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="N31" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="O31" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="P31" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="Q31" s="5" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.55000000000000004">
-      <c r="J32" s="5"/>
-      <c r="K32" s="5"/>
-      <c r="L32" s="5"/>
-      <c r="M32" s="5"/>
-      <c r="N32" s="5"/>
-      <c r="O32" s="5"/>
-      <c r="P32" s="5"/>
-      <c r="Q32" s="5"/>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" t="s">
-        <v>246</v>
-      </c>
-      <c r="J33" s="5"/>
-      <c r="K33" s="5"/>
-      <c r="L33" s="5"/>
-      <c r="M33" s="5"/>
-      <c r="N33" s="5"/>
-      <c r="O33" s="5"/>
-      <c r="P33" s="5"/>
-      <c r="Q33" s="5"/>
-      <c r="S33" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" t="s">
-        <v>235</v>
-      </c>
-      <c r="B34" t="s">
-        <v>51</v>
-      </c>
-      <c r="C34" t="s">
-        <v>51</v>
-      </c>
-      <c r="D34">
-        <v>0</v>
-      </c>
-      <c r="E34">
-        <v>0</v>
-      </c>
-      <c r="F34">
-        <v>0</v>
-      </c>
-      <c r="G34">
-        <v>0</v>
-      </c>
-      <c r="H34">
-        <v>1</v>
-      </c>
-      <c r="I34">
-        <v>1</v>
-      </c>
-      <c r="J34" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="K34" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="L34" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="M34" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="N34" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="O34" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="P34" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="Q34" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="S34" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" t="s">
-        <v>236</v>
-      </c>
-      <c r="B35" t="s">
-        <v>51</v>
-      </c>
-      <c r="C35" t="s">
-        <v>51</v>
-      </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-      <c r="E35">
-        <v>0</v>
-      </c>
-      <c r="F35">
-        <v>0</v>
-      </c>
-      <c r="G35">
-        <v>0</v>
-      </c>
-      <c r="H35">
-        <v>1</v>
-      </c>
-      <c r="I35">
-        <v>1</v>
-      </c>
-      <c r="J35" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="K35" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="L35" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="M35" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="N35" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="O35" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="P35" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q35" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" t="s">
-        <v>234</v>
-      </c>
-      <c r="B36" t="s">
-        <v>51</v>
-      </c>
-      <c r="C36" t="s">
-        <v>51</v>
-      </c>
-      <c r="D36" t="s">
-        <v>23</v>
-      </c>
-      <c r="E36" t="s">
-        <v>101</v>
-      </c>
-      <c r="F36" t="s">
-        <v>101</v>
-      </c>
-      <c r="G36" t="s">
-        <v>101</v>
-      </c>
-      <c r="H36" t="s">
-        <v>101</v>
-      </c>
-      <c r="I36" t="s">
-        <v>101</v>
-      </c>
-      <c r="J36" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="K36" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="L36" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="M36" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="N36" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="O36" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="P36" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q36" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="B38" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39">
-        <v>0</v>
-      </c>
-      <c r="B39" t="s">
-        <v>152</v>
-      </c>
-      <c r="D39" t="s">
-        <v>181</v>
-      </c>
-      <c r="E39" t="s">
-        <v>191</v>
-      </c>
-      <c r="I39" t="s">
-        <v>120</v>
-      </c>
-      <c r="L39" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40">
-        <v>1</v>
-      </c>
-      <c r="B40" t="s">
-        <v>153</v>
-      </c>
-      <c r="E40" t="s">
-        <v>191</v>
-      </c>
-      <c r="I40" t="s">
-        <v>43</v>
-      </c>
-      <c r="J40">
-        <v>8</v>
-      </c>
-      <c r="L40" t="s">
-        <v>46</v>
-      </c>
-      <c r="M40">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41">
-        <v>2</v>
-      </c>
-      <c r="B41" t="s">
-        <v>178</v>
-      </c>
-      <c r="I41" t="s">
-        <v>44</v>
-      </c>
-      <c r="J41">
-        <v>8</v>
-      </c>
-      <c r="L41" t="s">
-        <v>168</v>
-      </c>
-      <c r="M41" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42">
-        <v>3</v>
-      </c>
-      <c r="B42" t="s">
-        <v>162</v>
-      </c>
-      <c r="E42" t="s">
-        <v>191</v>
-      </c>
-      <c r="I42" t="s">
-        <v>165</v>
-      </c>
-      <c r="J42">
-        <v>4</v>
-      </c>
-      <c r="L42" t="s">
-        <v>169</v>
-      </c>
-      <c r="M42" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43">
-        <v>4</v>
-      </c>
-      <c r="B43" t="s">
-        <v>163</v>
-      </c>
-      <c r="E43" t="s">
-        <v>191</v>
-      </c>
-      <c r="I43" t="s">
-        <v>166</v>
-      </c>
-      <c r="J43">
-        <v>1</v>
-      </c>
-      <c r="L43" t="s">
-        <v>170</v>
-      </c>
-      <c r="M43" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44">
-        <v>5</v>
-      </c>
-      <c r="J44">
-        <f>SUM(J40:J43)</f>
-        <v>21</v>
-      </c>
-      <c r="K44">
-        <f>2^J44</f>
-        <v>2097152</v>
-      </c>
-      <c r="L44" t="s">
-        <v>171</v>
-      </c>
-      <c r="M44" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45">
-        <v>6</v>
-      </c>
-      <c r="B45" t="s">
-        <v>156</v>
-      </c>
-      <c r="D45" t="s">
-        <v>180</v>
-      </c>
-      <c r="L45" t="s">
-        <v>172</v>
-      </c>
-      <c r="M45" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46">
-        <v>7</v>
-      </c>
-      <c r="B46" t="s">
-        <v>154</v>
-      </c>
-      <c r="D46" t="s">
-        <v>192</v>
-      </c>
-      <c r="L46" t="s">
-        <v>173</v>
-      </c>
-      <c r="M46" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47">
-        <v>8</v>
-      </c>
-      <c r="B47" t="s">
-        <v>155</v>
-      </c>
-      <c r="D47" t="s">
-        <v>179</v>
-      </c>
-      <c r="L47" t="s">
-        <v>174</v>
-      </c>
-      <c r="M47" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48">
-        <v>9</v>
-      </c>
-      <c r="B48" t="s">
-        <v>157</v>
-      </c>
-      <c r="D48" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49">
-        <v>10</v>
-      </c>
-      <c r="B49" t="s">
-        <v>158</v>
-      </c>
-      <c r="D49" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50">
-        <v>11</v>
-      </c>
-      <c r="B50" t="s">
-        <v>159</v>
-      </c>
-      <c r="E50" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51">
-        <v>12</v>
-      </c>
-      <c r="B51" t="s">
-        <v>160</v>
-      </c>
-      <c r="E51" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52">
-        <v>13</v>
-      </c>
-      <c r="B52" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A53">
-        <v>14</v>
-      </c>
-      <c r="B53" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54">
-        <v>15</v>
-      </c>
-      <c r="B54" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="L57" t="s">
-        <v>187</v>
-      </c>
-      <c r="O57" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="B59">
-        <v>0</v>
-      </c>
-      <c r="C59">
-        <v>1</v>
-      </c>
-      <c r="D59">
-        <v>2</v>
-      </c>
-      <c r="E59">
-        <v>3</v>
-      </c>
-      <c r="F59">
-        <v>4</v>
-      </c>
-      <c r="G59">
-        <v>5</v>
-      </c>
-      <c r="H59">
-        <v>6</v>
-      </c>
-      <c r="I59">
-        <v>7</v>
-      </c>
-      <c r="J59">
-        <v>0</v>
-      </c>
-      <c r="K59">
-        <v>1</v>
-      </c>
-      <c r="L59">
-        <v>2</v>
-      </c>
-      <c r="M59">
-        <v>3</v>
-      </c>
-      <c r="N59">
-        <v>4</v>
-      </c>
-      <c r="O59">
-        <v>5</v>
-      </c>
-      <c r="P59">
-        <v>6</v>
-      </c>
-      <c r="Q59">
-        <v>7</v>
-      </c>
-      <c r="R59">
-        <v>0</v>
-      </c>
-      <c r="S59">
-        <v>1</v>
-      </c>
-      <c r="T59">
-        <v>2</v>
-      </c>
-      <c r="U59">
-        <v>3</v>
-      </c>
-      <c r="V59">
-        <v>4</v>
-      </c>
-      <c r="W59">
-        <v>5</v>
-      </c>
-      <c r="X59">
-        <v>6</v>
-      </c>
-      <c r="Y59">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="B60" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H60" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I60" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J60" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K60" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L60" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="M60" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="N60" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="O60" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P60" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q60" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A61" t="s">
-        <v>19</v>
-      </c>
-      <c r="B61" t="s">
-        <v>17</v>
-      </c>
-      <c r="C61" t="s">
-        <v>17</v>
-      </c>
-      <c r="D61" t="s">
-        <v>3</v>
-      </c>
-      <c r="E61" t="s">
-        <v>3</v>
-      </c>
-      <c r="F61" t="s">
-        <v>3</v>
-      </c>
-      <c r="G61" t="s">
-        <v>3</v>
-      </c>
-      <c r="H61" t="s">
-        <v>23</v>
-      </c>
-      <c r="I61" t="s">
-        <v>23</v>
-      </c>
-      <c r="J61" t="s">
-        <v>18</v>
-      </c>
-      <c r="K61" t="s">
-        <v>18</v>
-      </c>
-      <c r="L61" t="s">
-        <v>18</v>
-      </c>
-      <c r="M61" t="s">
-        <v>18</v>
-      </c>
-      <c r="N61" t="s">
-        <v>18</v>
-      </c>
-      <c r="O61" t="s">
-        <v>18</v>
-      </c>
-      <c r="P61" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q61" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A62" t="s">
-        <v>19</v>
-      </c>
-      <c r="B62" t="s">
-        <v>17</v>
-      </c>
-      <c r="C62" t="s">
-        <v>17</v>
-      </c>
-      <c r="D62" t="s">
-        <v>8</v>
-      </c>
-      <c r="E62" t="s">
-        <v>8</v>
-      </c>
-      <c r="F62" t="s">
-        <v>8</v>
-      </c>
-      <c r="G62" t="s">
-        <v>8</v>
-      </c>
-      <c r="H62" t="s">
-        <v>23</v>
-      </c>
-      <c r="I62" t="s">
-        <v>23</v>
-      </c>
-      <c r="J62" t="s">
-        <v>18</v>
-      </c>
-      <c r="K62" t="s">
-        <v>18</v>
-      </c>
-      <c r="L62" t="s">
-        <v>18</v>
-      </c>
-      <c r="M62" t="s">
-        <v>18</v>
-      </c>
-      <c r="N62" t="s">
-        <v>18</v>
-      </c>
-      <c r="O62" t="s">
-        <v>18</v>
-      </c>
-      <c r="P62" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q62" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A63" t="s">
-        <v>19</v>
-      </c>
-      <c r="B63" t="s">
-        <v>17</v>
-      </c>
-      <c r="C63" t="s">
-        <v>17</v>
-      </c>
-      <c r="D63" t="s">
-        <v>21</v>
-      </c>
-      <c r="E63" t="s">
-        <v>21</v>
-      </c>
-      <c r="F63" t="s">
-        <v>21</v>
-      </c>
-      <c r="G63" t="s">
-        <v>21</v>
-      </c>
-      <c r="H63" t="s">
-        <v>23</v>
-      </c>
-      <c r="I63" t="s">
-        <v>23</v>
-      </c>
-      <c r="J63" t="s">
-        <v>18</v>
-      </c>
-      <c r="K63" t="s">
-        <v>18</v>
-      </c>
-      <c r="L63" t="s">
-        <v>18</v>
-      </c>
-      <c r="M63" t="s">
-        <v>18</v>
-      </c>
-      <c r="N63" t="s">
-        <v>18</v>
-      </c>
-      <c r="O63" t="s">
-        <v>18</v>
-      </c>
-      <c r="P63" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q63" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="65" spans="1:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="A65" t="s">
-        <v>184</v>
-      </c>
-      <c r="B65" t="s">
-        <v>22</v>
-      </c>
-      <c r="C65" t="s">
-        <v>22</v>
-      </c>
-      <c r="D65" t="s">
-        <v>21</v>
-      </c>
-      <c r="E65" t="s">
-        <v>21</v>
-      </c>
-      <c r="F65" t="s">
-        <v>21</v>
-      </c>
-      <c r="G65" t="s">
-        <v>21</v>
-      </c>
-      <c r="H65" t="s">
-        <v>23</v>
-      </c>
-      <c r="I65" t="s">
-        <v>147</v>
-      </c>
-      <c r="J65" t="s">
-        <v>193</v>
-      </c>
-      <c r="K65" t="s">
-        <v>193</v>
-      </c>
-      <c r="L65" t="s">
-        <v>193</v>
-      </c>
-      <c r="M65" t="s">
-        <v>193</v>
-      </c>
-      <c r="N65" t="s">
-        <v>193</v>
-      </c>
-      <c r="O65" t="s">
-        <v>193</v>
-      </c>
-      <c r="P65" t="s">
-        <v>193</v>
-      </c>
-      <c r="Q65" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="66" spans="1:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="A66" t="s">
-        <v>148</v>
-      </c>
-      <c r="B66" t="s">
-        <v>22</v>
-      </c>
-      <c r="C66" t="s">
-        <v>22</v>
-      </c>
-      <c r="D66" t="s">
-        <v>21</v>
-      </c>
-      <c r="E66" t="s">
-        <v>21</v>
-      </c>
-      <c r="F66" t="s">
-        <v>21</v>
-      </c>
-      <c r="G66" t="s">
-        <v>21</v>
-      </c>
-      <c r="H66" t="s">
-        <v>23</v>
-      </c>
-      <c r="I66" t="s">
-        <v>146</v>
-      </c>
-      <c r="J66" t="s">
-        <v>23</v>
-      </c>
-      <c r="K66" t="s">
-        <v>23</v>
-      </c>
-      <c r="L66" t="s">
-        <v>23</v>
-      </c>
-      <c r="M66" t="s">
-        <v>23</v>
-      </c>
-      <c r="N66" t="s">
-        <v>23</v>
-      </c>
-      <c r="O66" t="s">
-        <v>23</v>
-      </c>
-      <c r="P66" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q66" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="68" spans="1:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="A68" t="s">
-        <v>55</v>
-      </c>
-      <c r="B68" t="s">
-        <v>24</v>
-      </c>
-      <c r="C68" t="s">
-        <v>24</v>
-      </c>
-      <c r="D68" t="s">
-        <v>3</v>
-      </c>
-      <c r="E68" t="s">
-        <v>3</v>
-      </c>
-      <c r="F68" t="s">
-        <v>3</v>
-      </c>
-      <c r="G68" t="s">
-        <v>3</v>
-      </c>
-      <c r="H68" t="s">
-        <v>34</v>
-      </c>
-      <c r="I68" t="s">
-        <v>34</v>
-      </c>
-      <c r="J68" t="s">
-        <v>34</v>
-      </c>
-      <c r="K68" t="s">
-        <v>34</v>
-      </c>
-      <c r="L68" t="s">
-        <v>15</v>
-      </c>
-      <c r="M68" t="s">
-        <v>15</v>
-      </c>
-      <c r="N68" t="s">
-        <v>15</v>
-      </c>
-      <c r="O68" t="s">
-        <v>16</v>
-      </c>
-      <c r="P68" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q68" t="s">
-        <v>16</v>
-      </c>
-      <c r="AA68" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="69" spans="1:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="A69" t="s">
-        <v>131</v>
-      </c>
-      <c r="B69" t="s">
-        <v>24</v>
-      </c>
-      <c r="C69" t="s">
-        <v>24</v>
-      </c>
-      <c r="D69" t="s">
-        <v>8</v>
-      </c>
-      <c r="E69" t="s">
-        <v>8</v>
-      </c>
-      <c r="F69" t="s">
-        <v>8</v>
-      </c>
-      <c r="G69" t="s">
-        <v>8</v>
-      </c>
-      <c r="H69" t="s">
-        <v>34</v>
-      </c>
-      <c r="I69" t="s">
-        <v>34</v>
-      </c>
-      <c r="J69" t="s">
-        <v>34</v>
-      </c>
-      <c r="K69" t="s">
-        <v>34</v>
-      </c>
-      <c r="L69" t="s">
-        <v>15</v>
-      </c>
-      <c r="M69" t="s">
-        <v>15</v>
-      </c>
-      <c r="N69" t="s">
-        <v>15</v>
-      </c>
-      <c r="O69" t="s">
-        <v>16</v>
-      </c>
-      <c r="P69" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q69" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="70" spans="1:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="A70" t="s">
-        <v>149</v>
-      </c>
-      <c r="B70" t="s">
-        <v>24</v>
-      </c>
-      <c r="C70" t="s">
-        <v>24</v>
-      </c>
-      <c r="D70" t="s">
-        <v>39</v>
-      </c>
-      <c r="E70" t="s">
-        <v>39</v>
-      </c>
-      <c r="F70" t="s">
-        <v>39</v>
-      </c>
-      <c r="G70" t="s">
-        <v>39</v>
-      </c>
-      <c r="H70" t="s">
-        <v>34</v>
-      </c>
-      <c r="I70" t="s">
-        <v>34</v>
-      </c>
-      <c r="J70" t="s">
-        <v>34</v>
-      </c>
-      <c r="K70" t="s">
-        <v>34</v>
-      </c>
-      <c r="L70" t="s">
-        <v>15</v>
-      </c>
-      <c r="M70" t="s">
-        <v>15</v>
-      </c>
-      <c r="N70" t="s">
-        <v>15</v>
-      </c>
-      <c r="O70" t="s">
-        <v>16</v>
-      </c>
-      <c r="P70" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q70" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="71" spans="1:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="A71" t="s">
-        <v>56</v>
-      </c>
-      <c r="B71" t="s">
-        <v>24</v>
-      </c>
-      <c r="C71" t="s">
-        <v>24</v>
-      </c>
-      <c r="D71" t="s">
-        <v>21</v>
-      </c>
-      <c r="E71" t="s">
-        <v>21</v>
-      </c>
-      <c r="F71" t="s">
-        <v>21</v>
-      </c>
-      <c r="G71" t="s">
-        <v>21</v>
-      </c>
-      <c r="H71" t="s">
-        <v>34</v>
-      </c>
-      <c r="I71" t="s">
-        <v>34</v>
-      </c>
-      <c r="J71" t="s">
-        <v>34</v>
-      </c>
-      <c r="K71" t="s">
-        <v>34</v>
-      </c>
-      <c r="L71" t="s">
-        <v>15</v>
-      </c>
-      <c r="M71" t="s">
-        <v>15</v>
-      </c>
-      <c r="N71" t="s">
-        <v>15</v>
-      </c>
-      <c r="O71" t="s">
-        <v>16</v>
-      </c>
-      <c r="P71" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q71" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="73" spans="1:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="A73" t="s">
-        <v>52</v>
-      </c>
-      <c r="B73" t="s">
-        <v>51</v>
-      </c>
-      <c r="C73" t="s">
-        <v>51</v>
-      </c>
-      <c r="D73" t="s">
-        <v>3</v>
-      </c>
-      <c r="E73" t="s">
-        <v>3</v>
-      </c>
-      <c r="F73" t="s">
-        <v>3</v>
-      </c>
-      <c r="G73" t="s">
-        <v>3</v>
-      </c>
-      <c r="H73" t="s">
-        <v>23</v>
-      </c>
-      <c r="I73" t="s">
-        <v>23</v>
-      </c>
-      <c r="J73" t="s">
-        <v>23</v>
-      </c>
-      <c r="K73" t="s">
-        <v>23</v>
-      </c>
-      <c r="L73" t="s">
-        <v>23</v>
-      </c>
-      <c r="M73" t="s">
-        <v>23</v>
-      </c>
-      <c r="N73" t="s">
-        <v>23</v>
-      </c>
-      <c r="O73" t="s">
-        <v>23</v>
-      </c>
-      <c r="P73" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q73" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="74" spans="1:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="A74" t="s">
-        <v>185</v>
-      </c>
-      <c r="B74" t="s">
-        <v>51</v>
-      </c>
-      <c r="C74" t="s">
-        <v>51</v>
-      </c>
-      <c r="D74" t="s">
-        <v>8</v>
-      </c>
-      <c r="E74" t="s">
-        <v>8</v>
-      </c>
-      <c r="F74" t="s">
-        <v>8</v>
-      </c>
-      <c r="G74" t="s">
-        <v>8</v>
-      </c>
-      <c r="H74" t="s">
-        <v>23</v>
-      </c>
-      <c r="I74" t="s">
-        <v>23</v>
-      </c>
-      <c r="J74" t="s">
-        <v>23</v>
-      </c>
-      <c r="K74" t="s">
-        <v>23</v>
-      </c>
-      <c r="L74" t="s">
-        <v>23</v>
-      </c>
-      <c r="M74" t="s">
-        <v>23</v>
-      </c>
-      <c r="N74" t="s">
-        <v>23</v>
-      </c>
-      <c r="O74" t="s">
-        <v>23</v>
-      </c>
-      <c r="P74" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q74" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="75" spans="1:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="A75" t="s">
-        <v>53</v>
-      </c>
-      <c r="B75" t="s">
-        <v>51</v>
-      </c>
-      <c r="C75" t="s">
-        <v>51</v>
-      </c>
-      <c r="D75" t="s">
-        <v>8</v>
-      </c>
-      <c r="E75" t="s">
-        <v>8</v>
-      </c>
-      <c r="F75" t="s">
-        <v>8</v>
-      </c>
-      <c r="G75" t="s">
-        <v>8</v>
-      </c>
-      <c r="I75" t="s">
-        <v>23</v>
-      </c>
-      <c r="J75" t="s">
-        <v>23</v>
-      </c>
-      <c r="K75" t="s">
-        <v>23</v>
-      </c>
-      <c r="L75" t="s">
-        <v>23</v>
-      </c>
-      <c r="M75" t="s">
-        <v>23</v>
-      </c>
-      <c r="N75" t="s">
-        <v>23</v>
-      </c>
-      <c r="O75" t="s">
-        <v>23</v>
-      </c>
-      <c r="P75" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q75" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="76" spans="1:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="A76" t="s">
-        <v>54</v>
-      </c>
-      <c r="B76" t="s">
-        <v>51</v>
-      </c>
-      <c r="C76" t="s">
-        <v>51</v>
-      </c>
-      <c r="D76" t="s">
-        <v>21</v>
-      </c>
-      <c r="E76" t="s">
-        <v>21</v>
-      </c>
-      <c r="F76" t="s">
-        <v>21</v>
-      </c>
-      <c r="G76" t="s">
-        <v>21</v>
-      </c>
-      <c r="I76" t="s">
-        <v>23</v>
-      </c>
-      <c r="J76" t="s">
-        <v>23</v>
-      </c>
-      <c r="K76" t="s">
-        <v>23</v>
-      </c>
-      <c r="L76" t="s">
-        <v>23</v>
-      </c>
-      <c r="M76" t="s">
-        <v>23</v>
-      </c>
-      <c r="N76" t="s">
-        <v>23</v>
-      </c>
-      <c r="O76" t="s">
-        <v>23</v>
-      </c>
-      <c r="P76" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q76" t="s">
-        <v>23</v>
-      </c>
+    <row r="51" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+      <c r="L51" s="1"/>
+      <c r="M51" s="1"/>
+      <c r="N51" s="1"/>
+      <c r="O51" s="1"/>
+      <c r="P51" s="1"/>
+      <c r="Q51" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7412,26 +6144,28 @@
   <dimension ref="A1:U34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="6" max="6" width="9.68359375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.62890625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.3125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.15625" customWidth="1"/>
     <col min="10" max="10" width="8.83984375" customWidth="1"/>
     <col min="16" max="16" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="K1" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -7468,13 +6202,10 @@
         <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G3" t="s">
-        <v>142</v>
+        <v>8</v>
       </c>
       <c r="K3" t="s">
-        <v>222</v>
+        <v>252</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -7497,7 +6228,7 @@
         <v>4</v>
       </c>
       <c r="K4" t="s">
-        <v>222</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -7520,7 +6251,7 @@
         <v>5</v>
       </c>
       <c r="K5" t="s">
-        <v>222</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -7540,13 +6271,10 @@
         <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" t="s">
-        <v>249</v>
+        <v>6</v>
       </c>
       <c r="K6" t="s">
-        <v>222</v>
+        <v>252</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -7566,10 +6294,13 @@
         <v>0</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
+      </c>
+      <c r="I7" t="s">
+        <v>249</v>
       </c>
       <c r="K7" t="s">
-        <v>222</v>
+        <v>252</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -7588,8 +6319,20 @@
       <c r="E8">
         <v>1</v>
       </c>
+      <c r="F8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>254</v>
+      </c>
+      <c r="H8" t="s">
+        <v>236</v>
+      </c>
+      <c r="I8" t="s">
+        <v>250</v>
+      </c>
       <c r="K8" t="s">
-        <v>222</v>
+        <v>252</v>
       </c>
       <c r="U8" t="s">
         <v>40</v>
@@ -7611,8 +6354,17 @@
       <c r="E9">
         <v>0</v>
       </c>
+      <c r="F9" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G9" t="s">
+        <v>204</v>
+      </c>
+      <c r="H9" t="s">
+        <v>251</v>
+      </c>
       <c r="K9" t="s">
-        <v>222</v>
+        <v>252</v>
       </c>
       <c r="U9" t="s">
         <v>40</v>
@@ -7634,9 +6386,17 @@
       <c r="E10">
         <v>1</v>
       </c>
-      <c r="F10" s="1"/>
+      <c r="F10" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="G10" t="s">
+        <v>134</v>
+      </c>
+      <c r="H10" t="s">
+        <v>251</v>
+      </c>
       <c r="K10" t="s">
-        <v>222</v>
+        <v>252</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -7656,16 +6416,16 @@
         <v>0</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>122</v>
+        <v>256</v>
       </c>
       <c r="G11" t="s">
-        <v>213</v>
+        <v>258</v>
       </c>
       <c r="H11" t="s">
-        <v>214</v>
+        <v>251</v>
       </c>
       <c r="K11" t="s">
-        <v>223</v>
+        <v>253</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -7685,19 +6445,16 @@
         <v>1</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>132</v>
+        <v>257</v>
       </c>
       <c r="G12" t="s">
-        <v>137</v>
+        <v>259</v>
       </c>
       <c r="H12" t="s">
-        <v>214</v>
+        <v>251</v>
       </c>
       <c r="K12" t="s">
-        <v>223</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>221</v>
+        <v>253</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -7717,19 +6474,16 @@
         <v>0</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G13" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="H13" t="s">
-        <v>214</v>
+        <v>251</v>
       </c>
       <c r="K13" t="s">
-        <v>223</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>221</v>
+        <v>253</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -7749,19 +6503,16 @@
         <v>1</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G14" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H14" t="s">
-        <v>214</v>
+        <v>251</v>
       </c>
       <c r="K14" t="s">
-        <v>223</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>221</v>
+        <v>253</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -7781,19 +6532,13 @@
         <v>0</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>135</v>
+        <v>245</v>
       </c>
       <c r="G15" t="s">
-        <v>139</v>
-      </c>
-      <c r="H15" t="s">
-        <v>214</v>
+        <v>260</v>
       </c>
       <c r="K15" t="s">
-        <v>223</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>221</v>
+        <v>253</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -7813,22 +6558,13 @@
         <v>1</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="G16" t="s">
-        <v>140</v>
-      </c>
-      <c r="H16" t="s">
-        <v>214</v>
+        <v>246</v>
       </c>
       <c r="K16" t="s">
-        <v>223</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>0</v>
       </c>
@@ -7845,16 +6581,13 @@
         <v>0</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="G17" t="s">
-        <v>143</v>
+        <v>247</v>
       </c>
       <c r="K17" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>0</v>
       </c>
@@ -7871,19 +6604,13 @@
         <v>1</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="G18" t="s">
-        <v>217</v>
-      </c>
-      <c r="H18" t="s">
-        <v>218</v>
+        <v>248</v>
       </c>
       <c r="K18" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="7">
         <v>1</v>
       </c>
@@ -7903,16 +6630,16 @@
         <v>43</v>
       </c>
       <c r="G19" t="s">
-        <v>141</v>
+        <v>137</v>
+      </c>
+      <c r="I19" t="s">
+        <v>262</v>
       </c>
       <c r="K19" t="s">
-        <v>224</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="7">
         <v>1</v>
       </c>
@@ -7932,13 +6659,13 @@
         <v>44</v>
       </c>
       <c r="G20" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="K20" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="7">
         <v>1</v>
       </c>
@@ -7958,13 +6685,13 @@
         <v>45</v>
       </c>
       <c r="G21" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="K21" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="7">
         <v>1</v>
       </c>
@@ -7984,13 +6711,13 @@
         <v>46</v>
       </c>
       <c r="G22" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="K22" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="7">
         <v>1</v>
       </c>
@@ -8010,13 +6737,13 @@
         <v>47</v>
       </c>
       <c r="G23" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="K23" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="7">
         <v>1</v>
       </c>
@@ -8036,13 +6763,13 @@
         <v>48</v>
       </c>
       <c r="G24" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="K24" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="7">
         <v>1</v>
       </c>
@@ -8062,13 +6789,13 @@
         <v>49</v>
       </c>
       <c r="G25" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="K25" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="7">
         <v>1</v>
       </c>
@@ -8088,13 +6815,13 @@
         <v>50</v>
       </c>
       <c r="G26" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="K26" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="7">
         <v>1</v>
       </c>
@@ -8111,16 +6838,16 @@
         <v>0</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="G27" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="K27" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="7">
         <v>1</v>
       </c>
@@ -8137,16 +6864,16 @@
         <v>1</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="G28" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="K28" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="7">
         <v>1</v>
       </c>
@@ -8163,16 +6890,16 @@
         <v>0</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="G29" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="K29" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="7">
         <v>1</v>
       </c>
@@ -8189,16 +6916,16 @@
         <v>1</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="G30" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="K30" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="7">
         <v>1</v>
       </c>
@@ -8215,16 +6942,16 @@
         <v>0</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="G31" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="K31" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="7">
         <v>1</v>
       </c>
@@ -8241,13 +6968,13 @@
         <v>1</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="G32" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="K32" t="s">
-        <v>224</v>
+        <v>261</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -8267,13 +6994,13 @@
         <v>0</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="G33" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="K33" t="s">
-        <v>224</v>
+        <v>261</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -8293,17 +7020,278 @@
         <v>1</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="G34" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="K34" t="s">
-        <v>224</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C272B348-F286-4209-8DF0-9430537DD256}">
+  <dimension ref="A2:G23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="1.68359375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.68359375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.68359375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.26171875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.1015625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.3125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="C2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>214</v>
+      </c>
+      <c r="C3" t="s">
+        <v>222</v>
+      </c>
+      <c r="D3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>215</v>
+      </c>
+      <c r="C4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D4" t="s">
+        <v>223</v>
+      </c>
+      <c r="E4" t="s">
+        <v>227</v>
+      </c>
+      <c r="F4" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D5" t="s">
+        <v>223</v>
+      </c>
+      <c r="E5" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" t="s">
+        <v>125</v>
+      </c>
+      <c r="G6" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" t="s">
+        <v>123</v>
+      </c>
+      <c r="E7" t="s">
+        <v>227</v>
+      </c>
+      <c r="F7" t="s">
+        <v>228</v>
+      </c>
+      <c r="G7" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>232</v>
+      </c>
+      <c r="C8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" t="s">
+        <v>123</v>
+      </c>
+      <c r="E8" t="s">
+        <v>229</v>
+      </c>
+      <c r="G8" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>217</v>
+      </c>
+      <c r="C9" t="s">
+        <v>126</v>
+      </c>
+      <c r="D9" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>218</v>
+      </c>
+      <c r="C10" t="s">
+        <v>126</v>
+      </c>
+      <c r="D10" t="s">
+        <v>123</v>
+      </c>
+      <c r="E10" t="s">
+        <v>227</v>
+      </c>
+      <c r="F10" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>213</v>
+      </c>
+      <c r="C11" t="s">
+        <v>126</v>
+      </c>
+      <c r="D11" t="s">
+        <v>123</v>
+      </c>
+      <c r="E11" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B13" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>239</v>
+      </c>
+      <c r="C17" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B21" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B22" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B23" t="s">
+        <v>244</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
basic alu working and control
</commit_message>
<xml_diff>
--- a/docs/SPAM1-AVR-Like.xlsx
+++ b/docs/SPAM1-AVR-Like.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/db8094ce4aaa691d/simplecpu/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="722" documentId="8_{E355E389-9FB3-4E8C-984E-0F784E421D7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{81650D60-A390-4370-AE38-1D3A2E243F85}"/>
+  <xr:revisionPtr revIDLastSave="1078" documentId="8_{E355E389-9FB3-4E8C-984E-0F784E421D7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{05C842B8-C76B-44D0-931C-C1BEB80BFC55}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" activeTab="3" xr2:uid="{B4484DA9-D572-4854-B84C-0917FAD72649}"/>
+    <workbookView xWindow="-48" yWindow="-48" windowWidth="23136" windowHeight="13056" activeTab="4" xr2:uid="{B4484DA9-D572-4854-B84C-0917FAD72649}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1443" uniqueCount="309">
   <si>
     <t>PCLOin</t>
   </si>
@@ -761,9 +761,6 @@
   </si>
   <si>
     <t>ZP_MODE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">implies write RAM select ZP, ALUOP=PASSX </t>
   </si>
   <si>
     <t>ROM_TO_DEVICE</t>
@@ -933,12 +930,117 @@
   <si>
     <t>implies OVERRIDE device and use write RAM, ZP=enable, ALUOP=PASSX (alu op 1),  REG_in=disable,</t>
   </si>
+  <si>
+    <t>implies write RAM select ZP</t>
+  </si>
+  <si>
+    <t>CHANGE ALUOP 0 to PASSX - SO A DISABLED BUFFER WITH PULL DOWNS CAN MUX IN THE "force ALUOP=0" CONTROL</t>
+  </si>
+  <si>
+    <t>RAM[ZP]=REGX</t>
+  </si>
+  <si>
+    <t>NONREG</t>
+  </si>
+  <si>
+    <t>NEED SOMETHING LIKETHIS  TO GET BACK TO 5 ALUOP BITS</t>
+  </si>
+  <si>
+    <t>DEV0</t>
+  </si>
+  <si>
+    <t>DEV1</t>
+  </si>
+  <si>
+    <t>DEV2</t>
+  </si>
+  <si>
+    <t>DEV3</t>
+  </si>
+  <si>
+    <t>DEV4/ALU</t>
+  </si>
+  <si>
+    <t>OP0</t>
+  </si>
+  <si>
+    <t>OP1</t>
+  </si>
+  <si>
+    <t>OP2</t>
+  </si>
+  <si>
+    <t>CONST</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>USE THIS ….</t>
+  </si>
+  <si>
+    <t>thought</t>
+  </si>
+  <si>
+    <t>&lt;&lt; if dev above is selected specifically with 00000 or 11111 then we can use these 13 bits for other perhaps …............................................&gt;&gt;</t>
+  </si>
+  <si>
+    <t>no way to do RAM[ZP]=ROM ?? :(   perhaps use bits [4:0]!=11111 as a const 0-31 to write into the ZP location to partially compensate for lack - those will be fairly common I expect</t>
+  </si>
+  <si>
+    <t>1 (0 illegal)</t>
+  </si>
+  <si>
+    <t>PASSX</t>
+  </si>
+  <si>
+    <t>REGX VAL</t>
+  </si>
+  <si>
+    <t>@OP</t>
+  </si>
+  <si>
+    <t>REGX ADDR</t>
+  </si>
+  <si>
+    <t>xxx</t>
+  </si>
+  <si>
+    <t>REGY ADDR</t>
+  </si>
+  <si>
+    <t>DEVY</t>
+  </si>
+  <si>
+    <t>DEVX</t>
+  </si>
+  <si>
+    <t>@DEVX</t>
+  </si>
+  <si>
+    <t>to ZP BUFFER</t>
+  </si>
+  <si>
+    <t>HARDWIRING …..........</t>
+  </si>
+  <si>
+    <t>REGXADDR</t>
+  </si>
+  <si>
+    <t>REGYADDR</t>
+  </si>
+  <si>
+    <t>toALU</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -967,8 +1069,40 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="8" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1005,6 +1139,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1018,7 +1164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -1030,6 +1176,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5348,96 +5503,95 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED8E6E0D-D3C4-4F44-A896-D8576BD5D307}">
-  <dimension ref="A1:Q51"/>
+  <dimension ref="A1:V54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.26171875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="40.68359375" customWidth="1"/>
-    <col min="2" max="17" width="8.83984375" customWidth="1"/>
+    <col min="2" max="2" width="27.47265625" customWidth="1"/>
+    <col min="3" max="18" width="6.89453125" customWidth="1"/>
+    <col min="19" max="20" width="7.5234375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.5234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="F1" t="s">
-        <v>269</v>
-      </c>
-      <c r="J1" t="s">
+    <row r="1" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="G1" t="s">
+        <v>268</v>
+      </c>
+      <c r="K1" t="s">
+        <v>266</v>
+      </c>
+      <c r="O1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="2" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="K2" t="s">
         <v>267</v>
       </c>
-      <c r="N1" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="J2" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4">
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="C4">
         <v>7</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>6</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>5</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>4</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>3</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>2</v>
       </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
       <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4" s="5">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4" s="5">
         <v>7</v>
       </c>
-      <c r="K4" s="5">
+      <c r="L4" s="5">
         <v>6</v>
       </c>
-      <c r="L4" s="5">
+      <c r="M4" s="5">
         <v>5</v>
       </c>
-      <c r="M4" s="5">
+      <c r="N4" s="5">
         <v>4</v>
       </c>
-      <c r="N4" s="5">
+      <c r="O4" s="5">
         <v>3</v>
       </c>
-      <c r="O4" s="5">
+      <c r="P4" s="5">
         <v>2</v>
       </c>
-      <c r="P4" s="5">
-        <v>1</v>
-      </c>
       <c r="Q4" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" s="1" t="s">
-        <v>221</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="R4" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.55000000000000004">
       <c r="C5" s="1" t="s">
         <v>221</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>101</v>
@@ -5451,8 +5605,8 @@
       <c r="I5" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="J5" s="8" t="s">
-        <v>41</v>
+      <c r="J5" s="1" t="s">
+        <v>101</v>
       </c>
       <c r="K5" s="8" t="s">
         <v>41</v>
@@ -5475,22 +5629,22 @@
       <c r="Q5" s="8" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
+      <c r="R5" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" t="s">
         <v>207</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>101</v>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>101</v>
@@ -5504,8 +5658,8 @@
       <c r="I6" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="J6" s="5" t="s">
-        <v>18</v>
+      <c r="J6" s="9" t="s">
+        <v>101</v>
       </c>
       <c r="K6" s="5" t="s">
         <v>18</v>
@@ -5528,25 +5682,27 @@
       <c r="Q6" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
+      <c r="R6" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="10">
-        <v>1</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>266</v>
-      </c>
-      <c r="F7" s="9"/>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="10">
+        <v>0</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>265</v>
+      </c>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
-      <c r="J7" s="5"/>
+      <c r="J7" s="9"/>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
@@ -5554,19 +5710,17 @@
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B9" s="1" t="s">
-        <v>221</v>
-      </c>
+      <c r="R7" s="5"/>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.55000000000000004">
       <c r="C9" s="1" t="s">
         <v>221</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>101</v>
@@ -5580,22 +5734,22 @@
       <c r="I9" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
+      <c r="J9" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B10" t="s">
         <v>234</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
       </c>
       <c r="C10" t="s">
         <v>22</v>
       </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>101</v>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>101</v>
@@ -5609,8 +5763,8 @@
       <c r="I10" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="J10" s="5" t="s">
-        <v>23</v>
+      <c r="J10" s="9" t="s">
+        <v>101</v>
       </c>
       <c r="K10" s="5" t="s">
         <v>23</v>
@@ -5633,22 +5787,22 @@
       <c r="Q10" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
+      <c r="R10" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B11" t="s">
         <v>235</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
       </c>
       <c r="C11" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="10">
-        <v>1</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>101</v>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="10">
+        <v>0</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>101</v>
@@ -5662,8 +5816,8 @@
       <c r="I11" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="J11" s="5" t="s">
-        <v>208</v>
+      <c r="J11" s="9" t="s">
+        <v>101</v>
       </c>
       <c r="K11" s="5" t="s">
         <v>208</v>
@@ -5686,33 +5840,38 @@
       <c r="Q11" s="5" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" t="s">
-        <v>22</v>
-      </c>
+      <c r="R11" s="5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.55000000000000004">
       <c r="C12" t="s">
         <v>22</v>
       </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B15" s="1" t="s">
-        <v>221</v>
-      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" ht="20.399999999999999" x14ac:dyDescent="0.75">
+      <c r="C14" s="11" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.55000000000000004">
       <c r="C15" s="1" t="s">
         <v>221</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>101</v>
@@ -5726,107 +5885,107 @@
       <c r="I15" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" t="s">
-        <v>273</v>
-      </c>
+      <c r="J15" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" t="s">
-        <v>24</v>
+        <v>263</v>
       </c>
       <c r="C16" t="s">
         <v>24</v>
       </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16" s="9">
-        <v>0</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>101</v>
+      <c r="D16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="10">
+        <v>0</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>101</v>
+        <v>210</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>101</v>
+        <v>210</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="J16" s="5" t="s">
-        <v>34</v>
+        <v>210</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>210</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>34</v>
+        <v>208</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>34</v>
+        <v>208</v>
       </c>
       <c r="M16" s="5" t="s">
-        <v>34</v>
+        <v>208</v>
       </c>
       <c r="N16" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="O16" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="P16" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Q16" s="5" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B17" s="1" t="s">
-        <v>24</v>
-      </c>
+        <v>208</v>
+      </c>
+      <c r="R16" s="5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.55000000000000004">
       <c r="C17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="1">
-        <v>0</v>
+      <c r="D17" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="E17" s="1">
         <v>0</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B18" t="s">
         <v>272</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" t="s">
-        <v>263</v>
-      </c>
-      <c r="B18" t="s">
-        <v>24</v>
       </c>
       <c r="C18" t="s">
         <v>24</v>
       </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18" s="9">
-        <v>1</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>210</v>
+      <c r="D18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18" s="9">
+        <v>0</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>210</v>
+        <v>101</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>210</v>
+        <v>101</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="J18" s="5" t="s">
-        <v>34</v>
+        <v>101</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>101</v>
       </c>
       <c r="K18" s="5" t="s">
         <v>34</v>
@@ -5838,7 +5997,7 @@
         <v>34</v>
       </c>
       <c r="N18" s="5" t="s">
-        <v>209</v>
+        <v>34</v>
       </c>
       <c r="O18" s="5" t="s">
         <v>209</v>
@@ -5849,42 +6008,42 @@
       <c r="Q18" s="5" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B19" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="R18" s="5" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.55000000000000004">
       <c r="C19" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="1">
-        <v>0</v>
+      <c r="D19" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="E19" s="1">
         <v>1</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+      <c r="G19" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" t="s">
-        <v>264</v>
-      </c>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" t="s">
-        <v>24</v>
+        <v>262</v>
       </c>
       <c r="C20" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="10">
-        <v>1</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>210</v>
+      <c r="D20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" s="9">
+        <v>1</v>
       </c>
       <c r="G20" s="9" t="s">
         <v>210</v>
@@ -5895,74 +6054,77 @@
       <c r="I20" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="J20" s="5" t="s">
-        <v>208</v>
+      <c r="J20" s="9" t="s">
+        <v>210</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>208</v>
+        <v>34</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>208</v>
+        <v>34</v>
       </c>
       <c r="M20" s="5" t="s">
-        <v>208</v>
+        <v>34</v>
       </c>
       <c r="N20" s="5" t="s">
-        <v>208</v>
+        <v>34</v>
       </c>
       <c r="O20" s="5" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="P20" s="5" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="Q20" s="5" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B21" s="1" t="s">
-        <v>24</v>
-      </c>
+        <v>209</v>
+      </c>
+      <c r="R20" s="5" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.55000000000000004">
       <c r="C21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="1">
-        <v>1</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F21" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B22" s="1"/>
+      <c r="D21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1</v>
+      </c>
+      <c r="F21" s="1">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B22" t="s">
+        <v>288</v>
+      </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="D24" s="1" t="s">
+      <c r="F22" s="1"/>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="E24" s="1" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" t="s">
+    <row r="25" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B25" t="s">
         <v>211</v>
-      </c>
-      <c r="B25" t="s">
-        <v>51</v>
       </c>
       <c r="C25" t="s">
         <v>51</v>
       </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25" t="s">
-        <v>101</v>
+      <c r="D25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
       </c>
       <c r="F25" t="s">
         <v>101</v>
@@ -5976,8 +6138,8 @@
       <c r="I25" t="s">
         <v>101</v>
       </c>
-      <c r="J25" s="5" t="s">
-        <v>23</v>
+      <c r="J25" t="s">
+        <v>101</v>
       </c>
       <c r="K25" s="5" t="s">
         <v>23</v>
@@ -6000,22 +6162,22 @@
       <c r="Q25" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" t="s">
+      <c r="R25" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B26" t="s">
         <v>213</v>
-      </c>
-      <c r="B26" t="s">
-        <v>51</v>
       </c>
       <c r="C26" t="s">
         <v>51</v>
       </c>
-      <c r="D26">
-        <v>0</v>
+      <c r="D26" t="s">
+        <v>51</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -6024,13 +6186,13 @@
         <v>0</v>
       </c>
       <c r="H26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I26">
         <v>1</v>
       </c>
-      <c r="J26" s="5" t="s">
-        <v>23</v>
+      <c r="J26">
+        <v>1</v>
       </c>
       <c r="K26" s="5" t="s">
         <v>23</v>
@@ -6053,21 +6215,21 @@
       <c r="Q26" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" t="s">
+      <c r="R26" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B27" t="s">
         <v>212</v>
-      </c>
-      <c r="B27" t="s">
-        <v>51</v>
       </c>
       <c r="C27" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="10">
-        <v>1</v>
-      </c>
-      <c r="E27">
+      <c r="D27" t="s">
+        <v>51</v>
+      </c>
+      <c r="E27" s="10">
         <v>0</v>
       </c>
       <c r="F27">
@@ -6077,13 +6239,13 @@
         <v>0</v>
       </c>
       <c r="H27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I27">
         <v>1</v>
       </c>
-      <c r="J27" s="5" t="s">
-        <v>208</v>
+      <c r="J27">
+        <v>1</v>
       </c>
       <c r="K27" s="5" t="s">
         <v>208</v>
@@ -6106,32 +6268,1093 @@
       <c r="Q27" s="5" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="E28" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="51" spans="2:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
-      <c r="I51" s="1"/>
-      <c r="J51" s="1"/>
-      <c r="K51" s="1"/>
-      <c r="L51" s="1"/>
-      <c r="M51" s="1"/>
-      <c r="N51" s="1"/>
-      <c r="O51" s="1"/>
-      <c r="P51" s="1"/>
-      <c r="Q51" s="1"/>
+      <c r="R27" s="5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="30" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="J30" s="16" t="s">
+        <v>304</v>
+      </c>
+      <c r="K30" s="16"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="7"/>
+      <c r="Q30" s="7"/>
+      <c r="R30" s="7"/>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="F31" s="18" t="s">
+        <v>305</v>
+      </c>
+      <c r="G31" s="18" t="s">
+        <v>305</v>
+      </c>
+      <c r="H31" s="18" t="s">
+        <v>305</v>
+      </c>
+      <c r="I31" s="18" t="s">
+        <v>305</v>
+      </c>
+      <c r="J31" s="18"/>
+      <c r="K31" s="17" t="s">
+        <v>303</v>
+      </c>
+      <c r="L31" s="17" t="s">
+        <v>303</v>
+      </c>
+      <c r="M31" s="17" t="s">
+        <v>303</v>
+      </c>
+      <c r="N31" s="17" t="s">
+        <v>303</v>
+      </c>
+      <c r="O31" s="17" t="s">
+        <v>303</v>
+      </c>
+      <c r="P31" s="17" t="s">
+        <v>303</v>
+      </c>
+      <c r="Q31" s="17" t="s">
+        <v>303</v>
+      </c>
+      <c r="R31" s="17" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B32" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="J32" s="19" t="s">
+        <v>307</v>
+      </c>
+      <c r="K32" s="19" t="s">
+        <v>307</v>
+      </c>
+      <c r="L32" s="19" t="s">
+        <v>307</v>
+      </c>
+      <c r="M32" s="19" t="s">
+        <v>307</v>
+      </c>
+      <c r="N32" s="19" t="s">
+        <v>307</v>
+      </c>
+      <c r="O32" s="18" t="s">
+        <v>306</v>
+      </c>
+      <c r="P32" s="18" t="s">
+        <v>306</v>
+      </c>
+      <c r="Q32" s="18" t="s">
+        <v>306</v>
+      </c>
+      <c r="R32" s="18" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34">
+        <v>0</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H34" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="I34" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="J34" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="K34" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="L34" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="M34" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="N34" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="O34" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="P34" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="Q34" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="R34" s="5" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="I35" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="J35" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="K35" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L35" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M35" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="N35" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="O35" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P35" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q35" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="R35" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36">
+        <v>2</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H36" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="I36" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="J36" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="K36" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="L36" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="M36" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="N36" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="O36" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="P36" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q36" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="R36" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="S36" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="T36" s="16" t="s">
+        <v>295</v>
+      </c>
+      <c r="U36" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="V36" s="5" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37">
+        <v>3</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="G37" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="H37" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="I37" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="J37" t="s">
+        <v>293</v>
+      </c>
+      <c r="K37" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="L37" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="M37" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="N37" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="O37" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="P37" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q37" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="R37" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="S37" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="T37" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="U37" s="14" t="s">
+        <v>301</v>
+      </c>
+      <c r="V37" s="5" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38">
+        <v>4</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="G38" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="H38" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="I38" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K38" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L38" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M38" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N38" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="O38" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="P38" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="Q38" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="R38" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="S38" s="15" t="s">
+        <v>296</v>
+      </c>
+      <c r="T38" s="7">
+        <v>0</v>
+      </c>
+      <c r="U38" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="V38" s="2" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39">
+        <v>5</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="G39" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="H39" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="I39" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K39" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L39" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M39" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N39" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="O39" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="P39" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="Q39" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="R39" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="S39" s="15" t="s">
+        <v>296</v>
+      </c>
+      <c r="T39" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="U39" s="14" t="s">
+        <v>301</v>
+      </c>
+      <c r="V39" s="5" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40">
+        <v>6</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="G40" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H40" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="I40" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="J40" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="K40" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L40" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M40" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="N40" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="O40" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P40" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q40" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="R40" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41">
+        <v>7</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41" t="s">
+        <v>23</v>
+      </c>
+      <c r="G41" t="s">
+        <v>23</v>
+      </c>
+      <c r="H41" t="s">
+        <v>23</v>
+      </c>
+      <c r="I41" t="s">
+        <v>23</v>
+      </c>
+      <c r="J41" t="s">
+        <v>23</v>
+      </c>
+      <c r="K41" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="L41" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="M41" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="N41" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="O41" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="P41" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q41" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="R41" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="B42" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="B43" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
+      <c r="L45" s="1"/>
+      <c r="M45" s="1"/>
+      <c r="N45" s="1"/>
+      <c r="O45" s="1"/>
+      <c r="P45" s="1"/>
+      <c r="Q45" s="1"/>
+      <c r="R45" s="1"/>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="B46" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="B47" t="s">
+        <v>207</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47" t="s">
+        <v>101</v>
+      </c>
+      <c r="G47" t="s">
+        <v>101</v>
+      </c>
+      <c r="H47" t="s">
+        <v>101</v>
+      </c>
+      <c r="I47" t="s">
+        <v>101</v>
+      </c>
+      <c r="J47" t="s">
+        <v>101</v>
+      </c>
+      <c r="K47" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="L47" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="M47" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="N47" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="O47" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="P47" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q47" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="R47" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="B48" t="s">
+        <v>234</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48" t="s">
+        <v>101</v>
+      </c>
+      <c r="G48" t="s">
+        <v>101</v>
+      </c>
+      <c r="H48" t="s">
+        <v>101</v>
+      </c>
+      <c r="I48" t="s">
+        <v>101</v>
+      </c>
+      <c r="J48" t="s">
+        <v>101</v>
+      </c>
+      <c r="K48" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L48" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M48" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="N48" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="O48" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P48" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q48" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="R48" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B49" t="s">
+        <v>235</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49" t="s">
+        <v>101</v>
+      </c>
+      <c r="G49" t="s">
+        <v>101</v>
+      </c>
+      <c r="H49" t="s">
+        <v>101</v>
+      </c>
+      <c r="I49" t="s">
+        <v>101</v>
+      </c>
+      <c r="J49" t="s">
+        <v>101</v>
+      </c>
+      <c r="K49" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="L49" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="M49" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="N49" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="O49" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="P49" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q49" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="R49" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="50" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B50" t="s">
+        <v>276</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50" t="s">
+        <v>23</v>
+      </c>
+      <c r="G50" t="s">
+        <v>210</v>
+      </c>
+      <c r="H50" t="s">
+        <v>210</v>
+      </c>
+      <c r="I50" t="s">
+        <v>210</v>
+      </c>
+      <c r="J50" t="s">
+        <v>210</v>
+      </c>
+      <c r="K50" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="L50" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="M50" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="N50" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="O50" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="P50" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q50" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="R50" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="51" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B51" t="s">
+        <v>272</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G51" t="s">
+        <v>277</v>
+      </c>
+      <c r="H51" t="s">
+        <v>277</v>
+      </c>
+      <c r="I51" t="s">
+        <v>277</v>
+      </c>
+      <c r="J51" t="s">
+        <v>277</v>
+      </c>
+      <c r="K51" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L51" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M51" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N51" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="O51" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="P51" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="Q51" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="R51" s="5" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="52" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B52" t="s">
+        <v>262</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G52" t="s">
+        <v>210</v>
+      </c>
+      <c r="H52" t="s">
+        <v>210</v>
+      </c>
+      <c r="I52" t="s">
+        <v>210</v>
+      </c>
+      <c r="J52" t="s">
+        <v>210</v>
+      </c>
+      <c r="K52" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L52" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M52" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N52" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="O52" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="P52" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="Q52" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="R52" s="5" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="53" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B53" t="s">
+        <v>211</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53" t="s">
+        <v>101</v>
+      </c>
+      <c r="G53" t="s">
+        <v>101</v>
+      </c>
+      <c r="H53" t="s">
+        <v>101</v>
+      </c>
+      <c r="I53" t="s">
+        <v>101</v>
+      </c>
+      <c r="J53" t="s">
+        <v>101</v>
+      </c>
+      <c r="K53" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L53" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M53" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="N53" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="O53" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P53" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q53" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="R53" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B54" t="s">
+        <v>218</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="F54" t="s">
+        <v>23</v>
+      </c>
+      <c r="G54" t="s">
+        <v>23</v>
+      </c>
+      <c r="H54" t="s">
+        <v>23</v>
+      </c>
+      <c r="I54" t="s">
+        <v>23</v>
+      </c>
+      <c r="J54" t="s">
+        <v>23</v>
+      </c>
+      <c r="K54" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="L54" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="M54" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="N54" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="O54" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="P54" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q54" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="R54" s="5" t="s">
+        <v>124</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6143,8 +7366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{327D4CAA-80C6-42B1-AA6F-3182C1F3C57C}">
   <dimension ref="A1:U34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -6205,7 +7428,7 @@
         <v>8</v>
       </c>
       <c r="K3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -6228,7 +7451,7 @@
         <v>4</v>
       </c>
       <c r="K4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -6251,7 +7474,7 @@
         <v>5</v>
       </c>
       <c r="K5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -6274,7 +7497,7 @@
         <v>6</v>
       </c>
       <c r="K6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -6297,10 +7520,10 @@
         <v>14</v>
       </c>
       <c r="I7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="K7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -6323,16 +7546,16 @@
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H8" t="s">
         <v>236</v>
       </c>
       <c r="I8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="K8" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="U8" t="s">
         <v>40</v>
@@ -6355,16 +7578,16 @@
         <v>0</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>122</v>
+        <v>308</v>
       </c>
       <c r="G9" t="s">
         <v>204</v>
       </c>
       <c r="H9" t="s">
+        <v>250</v>
+      </c>
+      <c r="K9" t="s">
         <v>251</v>
-      </c>
-      <c r="K9" t="s">
-        <v>252</v>
       </c>
       <c r="U9" t="s">
         <v>40</v>
@@ -6387,16 +7610,16 @@
         <v>1</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G10" t="s">
         <v>134</v>
       </c>
       <c r="H10" t="s">
+        <v>250</v>
+      </c>
+      <c r="K10" t="s">
         <v>251</v>
-      </c>
-      <c r="K10" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -6416,16 +7639,16 @@
         <v>0</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H11" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="K11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -6445,16 +7668,16 @@
         <v>1</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H12" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="K12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -6480,10 +7703,10 @@
         <v>135</v>
       </c>
       <c r="H13" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="K13" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -6509,10 +7732,10 @@
         <v>136</v>
       </c>
       <c r="H14" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="K14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -6532,13 +7755,13 @@
         <v>0</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K15" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -6558,10 +7781,10 @@
         <v>1</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="K16" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -6581,10 +7804,10 @@
         <v>0</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="K17" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -6604,10 +7827,10 @@
         <v>1</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="K18" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -6633,10 +7856,10 @@
         <v>137</v>
       </c>
       <c r="I19" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K19" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -6662,7 +7885,7 @@
         <v>137</v>
       </c>
       <c r="K20" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -6688,7 +7911,7 @@
         <v>137</v>
       </c>
       <c r="K21" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -6714,7 +7937,7 @@
         <v>137</v>
       </c>
       <c r="K22" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -6740,7 +7963,7 @@
         <v>137</v>
       </c>
       <c r="K23" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -6766,7 +7989,7 @@
         <v>137</v>
       </c>
       <c r="K24" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -6792,7 +8015,7 @@
         <v>137</v>
       </c>
       <c r="K25" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -6818,7 +8041,7 @@
         <v>137</v>
       </c>
       <c r="K26" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -6844,7 +8067,7 @@
         <v>137</v>
       </c>
       <c r="K27" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -6870,7 +8093,7 @@
         <v>137</v>
       </c>
       <c r="K28" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -6896,7 +8119,7 @@
         <v>137</v>
       </c>
       <c r="K29" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -6922,7 +8145,7 @@
         <v>137</v>
       </c>
       <c r="K30" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -6948,7 +8171,7 @@
         <v>137</v>
       </c>
       <c r="K31" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -6974,7 +8197,7 @@
         <v>137</v>
       </c>
       <c r="K32" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -7000,7 +8223,7 @@
         <v>137</v>
       </c>
       <c r="K33" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -7026,7 +8249,7 @@
         <v>137</v>
       </c>
       <c r="K34" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -7277,17 +8500,17 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
complex uart tx/rx works
</commit_message>
<xml_diff>
--- a/docs/SPAM1-AVR-Like.xlsx
+++ b/docs/SPAM1-AVR-Like.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/db8094ce4aaa691d/simplecpu/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1258" documentId="8_{E355E389-9FB3-4E8C-984E-0F784E421D7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9746110B-F562-4D97-802D-9A8AF7594C70}"/>
+  <xr:revisionPtr revIDLastSave="1314" documentId="8_{E355E389-9FB3-4E8C-984E-0F784E421D7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2ABA6115-9532-47D2-B380-BACF7666D41C}"/>
   <bookViews>
-    <workbookView xWindow="-48" yWindow="-48" windowWidth="23136" windowHeight="13056" activeTab="4" xr2:uid="{B4484DA9-D572-4854-B84C-0917FAD72649}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" activeTab="4" xr2:uid="{B4484DA9-D572-4854-B84C-0917FAD72649}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1624" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1612" uniqueCount="334">
   <si>
     <t>PCLOin</t>
   </si>
@@ -1152,12 +1152,18 @@
   <si>
     <t>where is a a reg</t>
   </si>
+  <si>
+    <t>XTO2</t>
+  </si>
+  <si>
+    <t>SPECIAL</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1226,6 +1232,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="8" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -1289,7 +1304,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -1310,6 +1325,8 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7553,8 +7570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B894701-19F4-4F50-851C-D12E2249ACA5}">
   <dimension ref="A3:X26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P11" sqref="L11:P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -7647,6 +7664,10 @@
       <c r="T5" s="18" t="s">
         <v>306</v>
       </c>
+      <c r="U5" s="20" t="s">
+        <v>333</v>
+      </c>
+      <c r="V5" s="18"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="D6" s="1"/>
@@ -7733,6 +7754,7 @@
       <c r="T7" s="5" t="s">
         <v>287</v>
       </c>
+      <c r="U7" s="1"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
@@ -7792,6 +7814,7 @@
       <c r="T8" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="U8" s="1"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
@@ -7851,18 +7874,10 @@
       <c r="T9" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="U9" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="V9" s="16" t="s">
-        <v>295</v>
-      </c>
-      <c r="W9" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="X9" s="5" t="s">
-        <v>299</v>
-      </c>
+      <c r="U9" s="16"/>
+      <c r="V9" s="16"/>
+      <c r="W9" s="5"/>
+      <c r="X9" s="5"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
@@ -7922,6 +7937,7 @@
       <c r="T10" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="U10" s="1"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
@@ -7981,18 +7997,12 @@
       <c r="T11" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="U11" s="15" t="s">
-        <v>296</v>
-      </c>
-      <c r="V11" s="7">
-        <v>0</v>
-      </c>
-      <c r="W11" s="5" t="s">
-        <v>298</v>
-      </c>
-      <c r="X11" s="2" t="s">
-        <v>300</v>
-      </c>
+      <c r="U11" s="21" t="s">
+        <v>332</v>
+      </c>
+      <c r="V11" s="7"/>
+      <c r="W11" s="5"/>
+      <c r="X11" s="2"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
@@ -8052,18 +8062,10 @@
       <c r="T12" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="U12" s="15" t="s">
-        <v>296</v>
-      </c>
-      <c r="V12" s="15" t="s">
-        <v>302</v>
-      </c>
-      <c r="W12" s="14" t="s">
-        <v>301</v>
-      </c>
-      <c r="X12" s="5" t="s">
-        <v>300</v>
-      </c>
+      <c r="U12" s="21"/>
+      <c r="V12" s="15"/>
+      <c r="W12" s="14"/>
+      <c r="X12" s="5"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
@@ -8123,18 +8125,12 @@
       <c r="T13" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="U13" s="7" t="s">
+      <c r="U13" s="16" t="s">
         <v>294</v>
       </c>
-      <c r="V13" s="15" t="s">
-        <v>302</v>
-      </c>
-      <c r="W13" s="14" t="s">
-        <v>301</v>
-      </c>
-      <c r="X13" s="5" t="s">
-        <v>298</v>
-      </c>
+      <c r="V13" s="15"/>
+      <c r="W13" s="14"/>
+      <c r="X13" s="5"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
@@ -8194,9 +8190,58 @@
       <c r="T14" s="5" t="s">
         <v>124</v>
       </c>
+      <c r="U14" s="1"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="D15" s="1"/>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="D16" s="1"/>

</xml_diff>